<commit_message>
Added function to write files for the CWE data to be put into graphs
</commit_message>
<xml_diff>
--- a/Graphs.xlsx
+++ b/Graphs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20730"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C939C5-4D70-4B94-86CC-8F124668F8B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E5F8CFE-97FA-454F-AC96-9F6E71EF114C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="2" r:id="rId1"/>
@@ -13,18 +13,9 @@
     <sheet name="Severity" sheetId="3" r:id="rId3"/>
     <sheet name="Vectors" sheetId="5" r:id="rId4"/>
     <sheet name="Complexity" sheetId="6" r:id="rId5"/>
+    <sheet name="CWE" sheetId="7" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlchart.v1.0" hidden="1">Data!$A$3:$A$18</definedName>
-    <definedName name="_xlchart.v1.1" hidden="1">Data!$B$2</definedName>
-    <definedName name="_xlchart.v1.2" hidden="1">Data!$B$3:$B$18</definedName>
-    <definedName name="_xlchart.v1.3" hidden="1">Data!$C$2</definedName>
-    <definedName name="_xlchart.v1.4" hidden="1">Data!$C$3:$C$18</definedName>
-    <definedName name="_xlchart.v1.5" hidden="1">Data!$A$3:$A$18</definedName>
-    <definedName name="_xlchart.v1.6" hidden="1">Data!$B$2</definedName>
-    <definedName name="_xlchart.v1.7" hidden="1">Data!$B$3:$B$18</definedName>
-    <definedName name="_xlchart.v1.8" hidden="1">Data!$C$2</definedName>
-    <definedName name="_xlchart.v1.9" hidden="1">Data!$C$3:$C$18</definedName>
     <definedName name="ExternalData_1" localSheetId="0" hidden="1">Data!$A$1:$L$18</definedName>
     <definedName name="ExternalData_2" localSheetId="0" hidden="1">Data!#REF!</definedName>
   </definedNames>
@@ -57,7 +48,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="51">
   <si>
     <t>Column1</t>
   </si>
@@ -163,6 +154,54 @@
   <si>
     <t>Neg Dev</t>
   </si>
+  <si>
+    <t>CWE-119</t>
+  </si>
+  <si>
+    <t>CWE-125</t>
+  </si>
+  <si>
+    <t>CWE-79</t>
+  </si>
+  <si>
+    <t>CWE-200</t>
+  </si>
+  <si>
+    <t>CWE-284</t>
+  </si>
+  <si>
+    <t>CWE-264</t>
+  </si>
+  <si>
+    <t>CWE-20</t>
+  </si>
+  <si>
+    <t>CWE-89</t>
+  </si>
+  <si>
+    <t>CWE-399</t>
+  </si>
+  <si>
+    <t>CWE-22</t>
+  </si>
+  <si>
+    <t>NVD-CWE-noinfo</t>
+  </si>
+  <si>
+    <t>NVD-CWE-Other</t>
+  </si>
+  <si>
+    <t>CWE-310</t>
+  </si>
+  <si>
+    <t>CWE-352</t>
+  </si>
+  <si>
+    <t>CWE-94</t>
+  </si>
+  <si>
+    <t>CWE-189</t>
+  </si>
 </sst>
 </file>
 
@@ -197,10 +236,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -10606,7 +10648,7 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N3" sqref="N3:N18"/>
+      <selection activeCell="H24" sqref="H24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11411,7 +11453,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5AF44E6-4337-42C1-B4D3-DEB78D4F83AD}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
@@ -11419,6 +11461,501 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36D64E2A-4335-4780-A6F3-F109F0F2F8A2}">
+  <dimension ref="A1:N11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="3">
+        <v>2011</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3">
+        <v>2012</v>
+      </c>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3">
+        <v>2013</v>
+      </c>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3">
+        <v>2014</v>
+      </c>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3">
+        <v>2015</v>
+      </c>
+      <c r="J1" s="3"/>
+      <c r="K1" s="3">
+        <v>2016</v>
+      </c>
+      <c r="L1" s="3"/>
+      <c r="M1" s="3">
+        <v>2017</v>
+      </c>
+      <c r="N1" s="3"/>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>728</v>
+      </c>
+      <c r="B2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C2">
+        <v>844</v>
+      </c>
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2">
+        <v>960</v>
+      </c>
+      <c r="F2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2">
+        <v>1547</v>
+      </c>
+      <c r="H2" t="s">
+        <v>47</v>
+      </c>
+      <c r="I2">
+        <v>1116</v>
+      </c>
+      <c r="J2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2">
+        <v>1363</v>
+      </c>
+      <c r="L2" t="s">
+        <v>35</v>
+      </c>
+      <c r="M2">
+        <v>2322</v>
+      </c>
+      <c r="N2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>536</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3">
+        <v>784</v>
+      </c>
+      <c r="D3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E3">
+        <v>774</v>
+      </c>
+      <c r="F3" t="s">
+        <v>35</v>
+      </c>
+      <c r="G3">
+        <v>948</v>
+      </c>
+      <c r="H3" t="s">
+        <v>37</v>
+      </c>
+      <c r="I3">
+        <v>776</v>
+      </c>
+      <c r="J3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K3">
+        <v>846</v>
+      </c>
+      <c r="L3" t="s">
+        <v>38</v>
+      </c>
+      <c r="M3">
+        <v>1274</v>
+      </c>
+      <c r="N3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>478</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="C4">
+        <v>680</v>
+      </c>
+      <c r="D4" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4">
+        <v>697</v>
+      </c>
+      <c r="F4" t="s">
+        <v>37</v>
+      </c>
+      <c r="G4">
+        <v>822</v>
+      </c>
+      <c r="H4" t="s">
+        <v>35</v>
+      </c>
+      <c r="I4">
+        <v>701</v>
+      </c>
+      <c r="J4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K4">
+        <v>788</v>
+      </c>
+      <c r="L4" t="s">
+        <v>45</v>
+      </c>
+      <c r="M4">
+        <v>1208</v>
+      </c>
+      <c r="N4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>451</v>
+      </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
+      <c r="C5">
+        <v>594</v>
+      </c>
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5">
+        <v>634</v>
+      </c>
+      <c r="F5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G5">
+        <v>709</v>
+      </c>
+      <c r="H5" t="s">
+        <v>45</v>
+      </c>
+      <c r="I5">
+        <v>648</v>
+      </c>
+      <c r="J5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K5">
+        <v>744</v>
+      </c>
+      <c r="L5" t="s">
+        <v>40</v>
+      </c>
+      <c r="M5">
+        <v>1175</v>
+      </c>
+      <c r="N5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>398</v>
+      </c>
+      <c r="B6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6">
+        <v>374</v>
+      </c>
+      <c r="D6" t="s">
+        <v>41</v>
+      </c>
+      <c r="E6">
+        <v>525</v>
+      </c>
+      <c r="F6" t="s">
+        <v>41</v>
+      </c>
+      <c r="G6">
+        <v>689</v>
+      </c>
+      <c r="H6" t="s">
+        <v>40</v>
+      </c>
+      <c r="I6">
+        <v>647</v>
+      </c>
+      <c r="J6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6">
+        <v>689</v>
+      </c>
+      <c r="L6" t="s">
+        <v>37</v>
+      </c>
+      <c r="M6">
+        <v>1023</v>
+      </c>
+      <c r="N6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>365</v>
+      </c>
+      <c r="B7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7">
+        <v>257</v>
+      </c>
+      <c r="D7" t="s">
+        <v>43</v>
+      </c>
+      <c r="E7">
+        <v>292</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7">
+        <v>509</v>
+      </c>
+      <c r="H7" t="s">
+        <v>41</v>
+      </c>
+      <c r="I7">
+        <v>577</v>
+      </c>
+      <c r="J7" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7">
+        <v>652</v>
+      </c>
+      <c r="L7" t="s">
+        <v>41</v>
+      </c>
+      <c r="M7">
+        <v>967</v>
+      </c>
+      <c r="N7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>321</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8">
+        <v>236</v>
+      </c>
+      <c r="D8" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8">
+        <v>261</v>
+      </c>
+      <c r="F8" t="s">
+        <v>38</v>
+      </c>
+      <c r="G8">
+        <v>418</v>
+      </c>
+      <c r="H8" t="s">
+        <v>38</v>
+      </c>
+      <c r="I8">
+        <v>545</v>
+      </c>
+      <c r="J8" t="s">
+        <v>41</v>
+      </c>
+      <c r="K8">
+        <v>584</v>
+      </c>
+      <c r="L8" t="s">
+        <v>39</v>
+      </c>
+      <c r="M8">
+        <v>459</v>
+      </c>
+      <c r="N8" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>208</v>
+      </c>
+      <c r="B9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C9">
+        <v>229</v>
+      </c>
+      <c r="D9" t="s">
+        <v>38</v>
+      </c>
+      <c r="E9">
+        <v>169</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9">
+        <v>349</v>
+      </c>
+      <c r="H9" t="s">
+        <v>46</v>
+      </c>
+      <c r="I9">
+        <v>352</v>
+      </c>
+      <c r="J9" t="s">
+        <v>43</v>
+      </c>
+      <c r="K9">
+        <v>304</v>
+      </c>
+      <c r="L9" t="s">
+        <v>46</v>
+      </c>
+      <c r="M9">
+        <v>374</v>
+      </c>
+      <c r="N9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>162</v>
+      </c>
+      <c r="B10" t="s">
+        <v>42</v>
+      </c>
+      <c r="C10">
+        <v>221</v>
+      </c>
+      <c r="D10" t="s">
+        <v>42</v>
+      </c>
+      <c r="E10">
+        <v>168</v>
+      </c>
+      <c r="F10" t="s">
+        <v>48</v>
+      </c>
+      <c r="G10">
+        <v>270</v>
+      </c>
+      <c r="H10" t="s">
+        <v>42</v>
+      </c>
+      <c r="I10">
+        <v>230</v>
+      </c>
+      <c r="J10" t="s">
+        <v>48</v>
+      </c>
+      <c r="K10">
+        <v>217</v>
+      </c>
+      <c r="L10" t="s">
+        <v>43</v>
+      </c>
+      <c r="M10">
+        <v>355</v>
+      </c>
+      <c r="N10" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>149</v>
+      </c>
+      <c r="B11" t="s">
+        <v>50</v>
+      </c>
+      <c r="C11">
+        <v>155</v>
+      </c>
+      <c r="D11" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11">
+        <v>160</v>
+      </c>
+      <c r="F11" t="s">
+        <v>49</v>
+      </c>
+      <c r="G11">
+        <v>269</v>
+      </c>
+      <c r="H11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I11">
+        <v>221</v>
+      </c>
+      <c r="J11" t="s">
+        <v>42</v>
+      </c>
+      <c r="K11">
+        <v>205</v>
+      </c>
+      <c r="L11" t="s">
+        <v>47</v>
+      </c>
+      <c r="M11">
+        <v>321</v>
+      </c>
+      <c r="N11" t="s">
+        <v>44</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="7">
+    <mergeCell ref="A1:B1"/>
+    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="I1:J1"/>
+    <mergeCell ref="K1:L1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
"Added last few CvssV2" metrics for graphing. Start refactoring to convert 8 lists to 1 list of objects. Goal is to help with looking at trends between metrics as well as general code readability.
</commit_message>
<xml_diff>
--- a/Graphs.xlsx
+++ b/Graphs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8E4FB22-8FF3-4344-B225-30BF2C594B36}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B17E8EE4-83FC-4D53-9F60-36BC205A1BC3}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4230,6 +4230,62 @@
               <a:effectLst/>
             </c:spPr>
           </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$A$3:$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2017</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
               <c:f>Data!$E$3:$E$18</c:f>
@@ -4309,27 +4365,6 @@
             <a:effectLst/>
           </c:spPr>
           <c:invertIfNegative val="0"/>
-          <c:dPt>
-            <c:idx val="14"/>
-            <c:invertIfNegative val="0"/>
-            <c:bubble3D val="0"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln>
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:extLst>
-              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                <c16:uniqueId val="{00000003-8FDA-4707-80E6-B8F5A7378D5D}"/>
-              </c:ext>
-            </c:extLst>
-          </c:dPt>
           <c:errBars>
             <c:errBarType val="both"/>
             <c:errValType val="stdErr"/>
@@ -4348,59 +4383,115 @@
               <a:effectLst/>
             </c:spPr>
           </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>Data!$A$3:$A$18</c:f>
+              <c:strCache>
+                <c:ptCount val="16"/>
+                <c:pt idx="0">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2015</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2016</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2017</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$G$3:$G$18</c:f>
+              <c:f>Data!$F$3:$F$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="16"/>
                 <c:pt idx="0">
-                  <c:v>4851</c:v>
+                  <c:v>3145</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1176</c:v>
+                  <c:v>692</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2180</c:v>
+                  <c:v>1066</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3898</c:v>
+                  <c:v>1863</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6353</c:v>
+                  <c:v>2948</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5809</c:v>
+                  <c:v>3114</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6363</c:v>
+                  <c:v>3501</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4406</c:v>
+                  <c:v>2241</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4246</c:v>
+                  <c:v>2172</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3823</c:v>
+                  <c:v>1781</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4574</c:v>
+                  <c:v>1712</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4780</c:v>
+                  <c:v>1871</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>5718</c:v>
+                  <c:v>2073</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6407</c:v>
+                  <c:v>2740</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7400</c:v>
+                  <c:v>3101</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11193</c:v>
+                  <c:v>3958</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -13433,7 +13524,7 @@
   <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="Q25" sqref="Q24:Q25"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14574,8 +14665,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40702091-B71B-41C0-BF10-F1E1694B8EC7}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S43" sqref="S43"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="S36" sqref="S36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14619,8 +14710,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36D64E2A-4335-4780-A6F3-F109F0F2F8A2}">
   <dimension ref="A1:Q97"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+    <sheetView topLeftCell="A8" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Added Slope and fixed some missing values
</commit_message>
<xml_diff>
--- a/Graphs.xlsx
+++ b/Graphs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F44068A-BE93-4201-90EE-D7F1F14AFDE4}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF16883D-C2AF-45F6-BDFE-DFCF51A5CD37}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="854" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="54">
   <si>
     <t>Column1</t>
   </si>
@@ -209,6 +209,18 @@
   </si>
   <si>
     <t>Total%</t>
+  </si>
+  <si>
+    <t>STD</t>
+  </si>
+  <si>
+    <t>STDEV</t>
+  </si>
+  <si>
+    <t>Slope</t>
+  </si>
+  <si>
+    <t>SLOPE</t>
   </si>
 </sst>
 </file>
@@ -2287,10 +2299,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Authentication!$P$4:$P$18</c:f>
+              <c:f>Authentication!$P$4:$P$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.99745012749362527</c:v>
                 </c:pt>
@@ -2335,6 +2347,9 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.85158601528131517</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.8453373768006065</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2438,10 +2453,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Authentication!$Q$4:$Q$18</c:f>
+              <c:f>Authentication!$Q$4:$Q$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>2.5498725063746812E-3</c:v>
                 </c:pt>
@@ -2486,6 +2501,9 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>0.14702477425329938</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.15466262319939347</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2589,10 +2607,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Authentication!$R$4:$R$18</c:f>
+              <c:f>Authentication!$R$4:$R$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2637,6 +2655,9 @@
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>1.3892104653855058E-3</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3603,10 +3624,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Confidentiality!$R$4:$R$17</c:f>
+              <c:f>Confidentiality!$R$4:$R$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.23383830808459577</c:v>
                 </c:pt>
@@ -3648,6 +3669,12 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.26054156001616596</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.27436906691363744</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.18324488248673237</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3733,10 +3760,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Confidentiality!$Q$4:$Q$17</c:f>
+              <c:f>Confidentiality!$Q$4:$Q$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.50457477126143691</c:v>
                 </c:pt>
@@ -3778,6 +3805,12 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.40899905698504646</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.40808057420699234</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.49590598938589842</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3863,10 +3896,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Confidentiality!$R$4:$R$17</c:f>
+              <c:f>Confidentiality!$R$4:$R$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.23383830808459577</c:v>
                 </c:pt>
@@ -3908,6 +3941,12 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.26054156001616596</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.27436906691363744</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.18324488248673237</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4892,10 +4931,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Integrity!$P$4:$P$17</c:f>
+              <c:f>Integrity!$P$4:$P$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.26158692065396733</c:v>
                 </c:pt>
@@ -4937,6 +4976,12 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.33045938299878758</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.31755035887937022</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.32084912812736921</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5022,10 +5067,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Integrity!$Q$4:$Q$17</c:f>
+              <c:f>Integrity!$Q$4:$Q$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.50457477126143691</c:v>
                 </c:pt>
@@ -5067,6 +5112,12 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.40899905698504646</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.40808057420699234</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.49590598938589842</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5152,10 +5203,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Integrity!$R$4:$R$17</c:f>
+              <c:f>Integrity!$R$4:$R$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="16"/>
                 <c:pt idx="0">
                   <c:v>0.23383830808459577</c:v>
                 </c:pt>
@@ -5197,6 +5248,12 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>0.26054156001616596</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.27436906691363744</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.18324488248673237</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -10319,7 +10376,17 @@
   <c:chart>
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.7120661204400939E-2"/>
+          <c:y val="4.6829206809777882E-2"/>
+          <c:w val="0.9185787667727181"/>
+          <c:h val="0.90634158638044426"/>
+        </c:manualLayout>
+      </c:layout>
       <c:barChart>
         <c:barDir val="col"/>
         <c:grouping val="clustered"/>
@@ -22908,14 +22975,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>468086</xdr:colOff>
       <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>483326</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>22266</xdr:rowOff>
     </xdr:to>
@@ -23027,16 +23094,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>215153</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>35859</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>230393</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>57101</xdr:rowOff>
+      <xdr:rowOff>92960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23109,15 +23176,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>403860</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:colOff>160020</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>53067</xdr:rowOff>
+      <xdr:colOff>175260</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>30207</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -23195,8 +23262,8 @@
       <xdr:rowOff>11430</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>129540</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>31</xdr:row>
       <xdr:rowOff>11430</xdr:rowOff>
     </xdr:to>
@@ -23268,16 +23335,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>143434</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>44823</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>15240</xdr:colOff>
-      <xdr:row>33</xdr:row>
-      <xdr:rowOff>182607</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>158674</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>48137</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -25260,10 +25327,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40702091-B71B-41C0-BF10-F1E1694B8EC7}">
-  <dimension ref="T3:X19"/>
+  <dimension ref="T3:X21"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X4" sqref="X4:X19"/>
+    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="W21" sqref="W21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -25635,6 +25702,40 @@
       <c r="X19">
         <f t="shared" si="0"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T20" t="s">
+        <v>51</v>
+      </c>
+      <c r="U20">
+        <f>STDEV(U6:U19)</f>
+        <v>2.5301491498118431E-2</v>
+      </c>
+      <c r="V20">
+        <f>STDEV(V6:V19)</f>
+        <v>5.2027988952339774E-2</v>
+      </c>
+      <c r="W20">
+        <f>STDEV(W6:W19)</f>
+        <v>6.9740793937465878E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="20:24" x14ac:dyDescent="0.3">
+      <c r="T21" t="s">
+        <v>52</v>
+      </c>
+      <c r="U21">
+        <f>SLOPE(U4:U19,Data!A4:A19)</f>
+        <v>1.585604014464462E-3</v>
+      </c>
+      <c r="V21">
+        <f>SLOPE(V4:V19,Data!B4:B19)</f>
+        <v>-0.11647307481095925</v>
+      </c>
+      <c r="W21">
+        <f>SLOPE(W4:W19,Data!C4:C19)</f>
+        <v>-0.11005039091948485</v>
       </c>
     </row>
   </sheetData>
@@ -25645,10 +25746,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DF78954-0FE9-4B8E-B491-EF82C601FC9E}">
-  <dimension ref="R3:V19"/>
+  <dimension ref="R3:V21"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U4" sqref="U4"/>
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26017,6 +26118,40 @@
       <c r="V19">
         <f t="shared" si="0"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="18:22" x14ac:dyDescent="0.3">
+      <c r="R20" t="s">
+        <v>51</v>
+      </c>
+      <c r="S20">
+        <f>STDEV(S6:S19)</f>
+        <v>4.8649953803729509E-2</v>
+      </c>
+      <c r="T20">
+        <f>STDEV(T6:T19)</f>
+        <v>4.8923267823787503E-2</v>
+      </c>
+      <c r="U20">
+        <f>STDEV(U6:U19)</f>
+        <v>2.7726606827552767E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="18:22" x14ac:dyDescent="0.3">
+      <c r="R21" t="s">
+        <v>53</v>
+      </c>
+      <c r="S21">
+        <f>SLOPE(S4:S19,Data!A4:A19)</f>
+        <v>1.9669824418775557E-3</v>
+      </c>
+      <c r="T21">
+        <f>SLOPE(T4:T19,Data!B4:B19)</f>
+        <v>-6.3668017010440128E-2</v>
+      </c>
+      <c r="U21">
+        <f>SLOPE(U4:U19,Data!C4:C19)</f>
+        <v>5.7516968039753737E-2</v>
       </c>
     </row>
   </sheetData>
@@ -26027,10 +26162,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A5AF44E6-4337-42C1-B4D3-DEB78D4F83AD}">
-  <dimension ref="R3:V19"/>
+  <dimension ref="R3:V21"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4:R19"/>
+      <selection activeCell="R22" sqref="R22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26399,6 +26534,40 @@
       <c r="V19">
         <f t="shared" si="0"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="18:22" x14ac:dyDescent="0.3">
+      <c r="R20" t="s">
+        <v>51</v>
+      </c>
+      <c r="S20">
+        <f>STDEV(S6:S19)</f>
+        <v>0.11614111900285479</v>
+      </c>
+      <c r="T20">
+        <f>STDEV(T6:T19)</f>
+        <v>0.12568989559337029</v>
+      </c>
+      <c r="U20">
+        <f>STDEV(U6:U19)</f>
+        <v>2.4760010149130755E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="18:22" x14ac:dyDescent="0.3">
+      <c r="R21" t="s">
+        <v>53</v>
+      </c>
+      <c r="S21">
+        <f>SLOPE(S4:S19,Data!C4:C19)</f>
+        <v>-0.17258800962550735</v>
+      </c>
+      <c r="T21">
+        <f>SLOPE(T4:T19,Data!C4:C19)</f>
+        <v>0.19769621794824535</v>
+      </c>
+      <c r="U21">
+        <f>SLOPE(U4:U19,Data!C4:C19)</f>
+        <v>-2.510820832273801E-2</v>
       </c>
     </row>
   </sheetData>
@@ -26410,10 +26579,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB7D030-842D-4660-9B07-FCA6FB1029BF}">
-  <dimension ref="O3:S18"/>
+  <dimension ref="O3:S21"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26453,7 +26622,7 @@
         <v>0</v>
       </c>
       <c r="S4">
-        <f t="shared" ref="S4:S18" si="0">P4+Q4+R4</f>
+        <f t="shared" ref="S4:S19" si="0">P4+Q4+R4</f>
         <v>1</v>
       </c>
     </row>
@@ -26763,6 +26932,62 @@
       <c r="S18">
         <f t="shared" si="0"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O19">
+        <f>dataset__6[[#This Row],[Column10]]+dataset__6[[#This Row],[Column11]]+dataset__6[[#This Row],[Column12]]</f>
+        <v>13190</v>
+      </c>
+      <c r="P19">
+        <f>dataset__6[[#This Row],[Column13]]/Authentication!O19</f>
+        <v>0.8453373768006065</v>
+      </c>
+      <c r="Q19">
+        <f>dataset__6[[#This Row],[Column14]]/Authentication!O19</f>
+        <v>0.15466262319939347</v>
+      </c>
+      <c r="R19">
+        <f>dataset__6[[#This Row],[Column15]]/Authentication!O19</f>
+        <v>0</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O20" t="s">
+        <v>51</v>
+      </c>
+      <c r="P20">
+        <f>STDEV(P5:P18)</f>
+        <v>5.4305858055819611E-2</v>
+      </c>
+      <c r="Q20">
+        <f>STDEV(Q5:Q18)</f>
+        <v>5.3665768841190759E-2</v>
+      </c>
+      <c r="R20">
+        <f>STDEV(R5:R18)</f>
+        <v>7.0252032945258619E-4</v>
+      </c>
+    </row>
+    <row r="21" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O21" t="s">
+        <v>53</v>
+      </c>
+      <c r="P21">
+        <f>SLOPE(P4:P19,Data!A4:A19)</f>
+        <v>-1.1679015013393176E-2</v>
+      </c>
+      <c r="Q21">
+        <f>SLOPE(Q4:Q19,Data!B4:B19)</f>
+        <v>-2.4761659809770586E-2</v>
+      </c>
+      <c r="R21">
+        <f>SLOPE(R4:R19,Data!C4:C19)</f>
+        <v>3.0305705528290696E-3</v>
       </c>
     </row>
   </sheetData>
@@ -26773,10 +26998,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F4246A9-8D0A-4820-BB45-BC5176DC873F}">
-  <dimension ref="O3:S17"/>
+  <dimension ref="O3:S21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+    <sheetView topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26816,7 +27041,7 @@
         <v>0.23383830808459577</v>
       </c>
       <c r="S4">
-        <f t="shared" ref="S4:S17" si="0">P4+Q4+R4</f>
+        <f t="shared" ref="S4:S18" si="0">P4+Q4+R4</f>
         <v>1</v>
       </c>
     </row>
@@ -27104,6 +27329,80 @@
       <c r="S17">
         <f t="shared" si="0"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O18">
+        <f>dataset__6[[#This Row],[Column10]]+dataset__6[[#This Row],[Column11]]+dataset__6[[#This Row],[Column12]]</f>
+        <v>8638</v>
+      </c>
+      <c r="P18">
+        <f>dataset__6[[#This Row],[Column16]]/Confidentiality!O18</f>
+        <v>0.31755035887937022</v>
+      </c>
+      <c r="Q18">
+        <f>dataset__6[[#This Row],[Column17]]/Confidentiality!O18</f>
+        <v>0.40808057420699234</v>
+      </c>
+      <c r="R18">
+        <f>dataset__6[[#This Row],[Column18]]/Confidentiality!O18</f>
+        <v>0.27436906691363744</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O19">
+        <f>dataset__6[[#This Row],[Column10]]+dataset__6[[#This Row],[Column11]]+dataset__6[[#This Row],[Column12]]</f>
+        <v>13190</v>
+      </c>
+      <c r="P19">
+        <f>dataset__6[[#This Row],[Column16]]/Confidentiality!O19</f>
+        <v>0.32084912812736921</v>
+      </c>
+      <c r="Q19">
+        <f>dataset__6[[#This Row],[Column17]]/Confidentiality!O19</f>
+        <v>0.49590598938589842</v>
+      </c>
+      <c r="R19">
+        <f>dataset__6[[#This Row],[Column18]]/Confidentiality!O19</f>
+        <v>0.18324488248673237</v>
+      </c>
+    </row>
+    <row r="20" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O20" t="s">
+        <v>50</v>
+      </c>
+      <c r="P20">
+        <f>STDEV(P4:P17)</f>
+        <v>4.0700145286531451E-2</v>
+      </c>
+      <c r="Q20">
+        <f>STDEV(Q4:Q17)</f>
+        <v>7.3902014233470495E-2</v>
+      </c>
+      <c r="R20">
+        <f>STDEV(R4:R17)</f>
+        <v>6.457305741626379E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O21" t="s">
+        <v>53</v>
+      </c>
+      <c r="P21">
+        <f>SLOPE(P4:P19,Data!C4:C19)</f>
+        <v>0.11690543407058659</v>
+      </c>
+      <c r="Q21">
+        <f>SLOPE(Q4:Q19,Data!C4:C19)</f>
+        <v>-0.4318748227829079</v>
+      </c>
+      <c r="R21">
+        <f>SLOPE(R4:R19,Data!C4:C19)</f>
+        <v>0.31496938871232133</v>
       </c>
     </row>
   </sheetData>
@@ -27114,10 +27413,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6F7C5608-D377-4F96-A309-68C8F0ACA5CD}">
-  <dimension ref="O3:S17"/>
+  <dimension ref="O3:S21"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P4" sqref="P4"/>
+    <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="P21" sqref="P21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27176,7 +27475,7 @@
         <v>0.17678452301534356</v>
       </c>
       <c r="S5">
-        <f t="shared" ref="S5:S17" si="0">P5+Q5+R5</f>
+        <f t="shared" ref="S5:S19" si="0">P5+Q5+R5</f>
         <v>1</v>
       </c>
     </row>
@@ -27442,6 +27741,84 @@
       <c r="S17">
         <f t="shared" si="0"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O18">
+        <f>dataset__6[[#This Row],[Column10]]+dataset__6[[#This Row],[Column11]]+dataset__6[[#This Row],[Column12]]</f>
+        <v>8638</v>
+      </c>
+      <c r="P18">
+        <f>dataset__6[[#This Row],[Column16]]/Confidentiality!O18</f>
+        <v>0.31755035887937022</v>
+      </c>
+      <c r="Q18">
+        <f>dataset__6[[#This Row],[Column17]]/Confidentiality!O18</f>
+        <v>0.40808057420699234</v>
+      </c>
+      <c r="R18">
+        <f>dataset__6[[#This Row],[Column18]]/Confidentiality!O18</f>
+        <v>0.27436906691363744</v>
+      </c>
+      <c r="S18">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O19">
+        <f>dataset__6[[#This Row],[Column10]]+dataset__6[[#This Row],[Column11]]+dataset__6[[#This Row],[Column12]]</f>
+        <v>13190</v>
+      </c>
+      <c r="P19">
+        <f>dataset__6[[#This Row],[Column16]]/Confidentiality!O19</f>
+        <v>0.32084912812736921</v>
+      </c>
+      <c r="Q19">
+        <f>dataset__6[[#This Row],[Column17]]/Confidentiality!O19</f>
+        <v>0.49590598938589842</v>
+      </c>
+      <c r="R19">
+        <f>dataset__6[[#This Row],[Column18]]/Confidentiality!O19</f>
+        <v>0.18324488248673237</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O20" t="s">
+        <v>51</v>
+      </c>
+      <c r="P20">
+        <f>STDEV(P4:P17)</f>
+        <v>4.0700145286531451E-2</v>
+      </c>
+      <c r="Q20">
+        <f>STDEV(Q4:Q17)</f>
+        <v>7.3902014233470495E-2</v>
+      </c>
+      <c r="R20">
+        <f>STDEV(R4:R17)</f>
+        <v>6.457305741626379E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O21" t="s">
+        <v>53</v>
+      </c>
+      <c r="P21">
+        <f>SLOPE(P4:P19,Data!C4:C19)</f>
+        <v>0.11690543407058659</v>
+      </c>
+      <c r="Q21">
+        <f>SLOPE(Q4:Q19,Data!C4:C19)</f>
+        <v>-0.4318748227829079</v>
+      </c>
+      <c r="R21">
+        <f>SLOPE(R4:R19,Data!C4:C19)</f>
+        <v>0.31496938871232133</v>
       </c>
     </row>
   </sheetData>
@@ -27452,10 +27829,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8915A04C-28DB-4189-A27F-575FCA82F4DD}">
-  <dimension ref="O3:S19"/>
+  <dimension ref="O3:S21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X25" sqref="X25"/>
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27824,6 +28201,40 @@
       <c r="S19">
         <f t="shared" si="0"/>
         <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O20" t="s">
+        <v>50</v>
+      </c>
+      <c r="P20">
+        <f>STDEV(P6:P19)</f>
+        <v>3.5509380866156411E-2</v>
+      </c>
+      <c r="Q20">
+        <f>STDEV(Q6:Q19)</f>
+        <v>7.2012705615197042E-2</v>
+      </c>
+      <c r="R20">
+        <f>STDEV(R6:R19)</f>
+        <v>6.6147662467760965E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="15:19" x14ac:dyDescent="0.3">
+      <c r="O21" t="s">
+        <v>53</v>
+      </c>
+      <c r="P21">
+        <f>SLOPE(P4:P19,Data!C4:C19)</f>
+        <v>0.11690543407058659</v>
+      </c>
+      <c r="Q21">
+        <f>SLOPE(Q4:Q19,Data!C4:C19)</f>
+        <v>-0.4318748227829079</v>
+      </c>
+      <c r="R21">
+        <f>SLOPE(R4:R19,Data!C4:C19)</f>
+        <v>0.31496938871232133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed slope calculation in a couple places where it was using the wrong column
</commit_message>
<xml_diff>
--- a/Graphs.xlsx
+++ b/Graphs.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20827"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF16883D-C2AF-45F6-BDFE-DFCF51A5CD37}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F3DF1B3-2B04-477C-BF6A-F1F7110BB8D6}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="854" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" tabRatio="854" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="10" r:id="rId1"/>
@@ -25329,7 +25329,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40702091-B71B-41C0-BF10-F1E1694B8EC7}">
   <dimension ref="T3:X21"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="W21" sqref="W21"/>
     </sheetView>
   </sheetViews>
@@ -25726,12 +25726,12 @@
         <v>52</v>
       </c>
       <c r="U21">
-        <f>SLOPE(U4:U19,Data!A4:A19)</f>
-        <v>1.585604014464462E-3</v>
+        <f>SLOPE(U4:U19,Data!C4:C19)</f>
+        <v>8.5638330481790551E-2</v>
       </c>
       <c r="V21">
-        <f>SLOPE(V4:V19,Data!B4:B19)</f>
-        <v>-0.11647307481095925</v>
+        <f>SLOPE(V4:V19,Data!C4:C19)</f>
+        <v>2.4412060437694377E-2</v>
       </c>
       <c r="W21">
         <f>SLOPE(W4:W19,Data!C4:C19)</f>
@@ -26142,12 +26142,12 @@
         <v>53</v>
       </c>
       <c r="S21">
-        <f>SLOPE(S4:S19,Data!A4:A19)</f>
-        <v>1.9669824418775557E-3</v>
+        <f>SLOPE(S4:S19,Data!C4:C19)</f>
+        <v>5.2461111937361872E-3</v>
       </c>
       <c r="T21">
-        <f>SLOPE(T4:T19,Data!B4:B19)</f>
-        <v>-6.3668017010440128E-2</v>
+        <f>SLOPE(T4:T19,Data!C4:C19)</f>
+        <v>-6.2763079233489921E-2</v>
       </c>
       <c r="U21">
         <f>SLOPE(U4:U19,Data!C4:C19)</f>
@@ -26165,7 +26165,7 @@
   <dimension ref="R3:V21"/>
   <sheetViews>
     <sheetView topLeftCell="A3" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R22" sqref="R22"/>
+      <selection activeCell="U21" sqref="U21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -26581,7 +26581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CB7D030-842D-4660-9B07-FCA6FB1029BF}">
   <dimension ref="O3:S21"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
+    <sheetView topLeftCell="A3" workbookViewId="0">
       <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
@@ -26978,12 +26978,12 @@
         <v>53</v>
       </c>
       <c r="P21">
-        <f>SLOPE(P4:P19,Data!A4:A19)</f>
-        <v>-1.1679015013393176E-2</v>
+        <f>SLOPE(P4:P19,Data!C4:C19)</f>
+        <v>-0.14806482419605516</v>
       </c>
       <c r="Q21">
-        <f>SLOPE(Q4:Q19,Data!B4:B19)</f>
-        <v>-2.4761659809770586E-2</v>
+        <f>SLOPE(Q4:Q19,Data!C4:C19)</f>
+        <v>0.14503425364322611</v>
       </c>
       <c r="R21">
         <f>SLOPE(R4:R19,Data!C4:C19)</f>
@@ -27001,7 +27001,7 @@
   <dimension ref="O3:S21"/>
   <sheetViews>
     <sheetView topLeftCell="B4" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27416,7 +27416,7 @@
   <dimension ref="O3:S21"/>
   <sheetViews>
     <sheetView topLeftCell="A4" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P21" sqref="P21"/>
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -27831,8 +27831,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8915A04C-28DB-4189-A27F-575FCA82F4DD}">
   <dimension ref="O3:S21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="R21" sqref="R21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>